<commit_message>
updted all four arcos files
</commit_message>
<xml_diff>
--- a/inputs/2018_arcos.xlsx
+++ b/inputs/2018_arcos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoselyncervantes/ml-fa21/ml-final/project_code/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E5DD62-D817-4144-9072-8DDFE8D3E86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A6BF9-0022-0441-8C60-744F6124EBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60620" yWindow="4520" windowWidth="14400" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31640" yWindow="900" windowWidth="34760" windowHeight="24900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -32,159 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
-  <si>
-    <t>ALABAMA TOTAL</t>
-  </si>
-  <si>
-    <t>ALASKA TOTAL</t>
-  </si>
-  <si>
-    <t>ARIZONA TOTAL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>ARKANSAS</t>
-  </si>
-  <si>
-    <t>CALIFORNIA TOTAL</t>
-  </si>
-  <si>
-    <t>COLORADO TOTAL</t>
-  </si>
-  <si>
-    <t>CONNECTICUT TOTAL</t>
-  </si>
-  <si>
-    <t>DELAWARE total</t>
-  </si>
-  <si>
-    <t>DC TOTAL</t>
-  </si>
-  <si>
-    <t>FLORIDA TOTAL</t>
-  </si>
-  <si>
-    <t>GEORGIA TOTAL</t>
-  </si>
-  <si>
-    <t>HAWAII TOTAL</t>
-  </si>
-  <si>
-    <t>IDAHO TOTAL</t>
-  </si>
-  <si>
-    <t>ILLINOIS TOTAL</t>
-  </si>
-  <si>
-    <t>INDIANA TOTAL</t>
-  </si>
-  <si>
-    <t>IOWA TOTAL</t>
-  </si>
-  <si>
-    <t>KANSAS TOTAL</t>
-  </si>
-  <si>
-    <t>KENTUCKY TOTAL</t>
-  </si>
-  <si>
-    <t>LOUSIANA TOTAL</t>
-  </si>
-  <si>
-    <t>MAINE TOTAL</t>
-  </si>
-  <si>
-    <t>MARYLAND TOTAL</t>
-  </si>
-  <si>
-    <t>MASSACHUSETTS TOTAL</t>
-  </si>
-  <si>
-    <t>MICHIGAN TOTAL</t>
-  </si>
-  <si>
-    <t>MINNISOTA TOTAL</t>
-  </si>
-  <si>
-    <t>MISSISSIPPI TOTAL</t>
-  </si>
-  <si>
-    <t>MISSOURI TOTAL</t>
-  </si>
-  <si>
-    <t>MONTANA TOTAL</t>
-  </si>
-  <si>
-    <t>NEBRASKA TOTAL</t>
-  </si>
-  <si>
-    <t>NEVADA TOTAL</t>
-  </si>
-  <si>
-    <t>NEW HAMPSHIRE TOTAL</t>
-  </si>
-  <si>
-    <t>NEW JERSEY TOTAL</t>
-  </si>
-  <si>
-    <t>NEW MEXICO TOTAL</t>
-  </si>
-  <si>
-    <t>NEW YORK TOTAL</t>
-  </si>
-  <si>
-    <t>NORTH CAROLINA TOTAL</t>
-  </si>
-  <si>
-    <t>NORTH DAKOTA TOTAL</t>
-  </si>
-  <si>
-    <t>OHIO TOTAL</t>
-  </si>
-  <si>
-    <t>OKLAHOMA TOTAL</t>
-  </si>
-  <si>
-    <t>OREGON TOTAL</t>
-  </si>
-  <si>
-    <t>PENNSYLVANIA TOTAL</t>
-  </si>
-  <si>
-    <t>RHODE ISLAND TOTAL</t>
-  </si>
-  <si>
-    <t>SOUTH CAROLINA TOTAL</t>
-  </si>
-  <si>
-    <t>SOUTH DAKOTA TOTAL</t>
-  </si>
-  <si>
-    <t>TENNESSEE TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEXAS TOTAL </t>
-  </si>
-  <si>
-    <t>UTAH TOTAL</t>
-  </si>
-  <si>
-    <t>VERMONT TOTAL</t>
-  </si>
-  <si>
-    <t>VIRGINIA TOTAL</t>
-  </si>
-  <si>
-    <t>WASHINGTON TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WEST VIRGINIA TOTAL</t>
-  </si>
-  <si>
-    <t>WISCONSIN TOTAL</t>
-  </si>
-  <si>
-    <t>WYOMING TOTAL</t>
   </si>
   <si>
     <t>STATE</t>
@@ -192,12 +42,165 @@
   <si>
     <t>TOTAL GRAMS</t>
   </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALABAMA </t>
+  </si>
+  <si>
+    <t>DISTRICT OF COLUMBIA</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>ALASKA</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>CONNECTICUT</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>IDAHO</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>IOWA</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>KENTUCKY</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>MAINE</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>MONTANA</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>NEW HAMPSHIRE</t>
+  </si>
+  <si>
+    <t>NEW JERSEY</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>NORTH DAKOTA</t>
+  </si>
+  <si>
+    <t>OHIO</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>RHODE ISLAND</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>SOUTH DAKOTA</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>VERMONT</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>WISCONSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WYOMING </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -205,10 +208,17 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
+      <name val="Cambria"/>
       <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,30 +241,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -271,8 +275,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -329,8 +333,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -387,8 +391,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -445,8 +449,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -503,8 +507,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -561,8 +565,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -619,8 +623,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -677,8 +681,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -735,8 +739,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -793,8 +797,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -851,8 +855,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -909,8 +913,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -967,8 +971,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1025,8 +1029,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1083,8 +1087,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1141,8 +1145,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1199,8 +1203,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1257,8 +1261,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1315,8 +1319,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1373,8 +1377,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1431,8 +1435,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1489,8 +1493,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1547,8 +1551,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1605,8 +1609,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1663,8 +1667,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1721,8 +1725,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1779,8 +1783,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1837,8 +1841,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1895,8 +1899,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1953,8 +1957,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2011,8 +2015,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2069,8 +2073,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2127,8 +2131,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2185,8 +2189,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2243,8 +2247,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2301,8 +2305,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2359,8 +2363,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2417,8 +2421,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2475,8 +2479,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2533,8 +2537,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2591,8 +2595,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2649,8 +2653,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2707,8 +2711,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2765,8 +2769,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2823,8 +2827,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2881,8 +2885,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2939,8 +2943,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2997,8 +3001,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3055,8 +3059,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3113,8 +3117,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3171,8 +3175,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3229,8 +3233,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3287,8 +3291,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3345,8 +3349,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3403,8 +3407,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3461,8 +3465,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3519,8 +3523,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3577,8 +3581,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3635,8 +3639,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3693,8 +3697,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3751,8 +3755,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3809,8 +3813,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3867,8 +3871,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3925,8 +3929,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -3983,8 +3987,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4041,8 +4045,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4099,8 +4103,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4157,8 +4161,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4215,8 +4219,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4273,8 +4277,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4331,8 +4335,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4389,8 +4393,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4447,8 +4451,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4505,8 +4509,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4563,8 +4567,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>463295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4621,8 +4625,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4679,8 +4683,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4737,8 +4741,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4795,8 +4799,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4853,8 +4857,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4911,8 +4915,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4969,8 +4973,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5027,8 +5031,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5085,8 +5089,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5143,8 +5147,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5201,8 +5205,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5259,8 +5263,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5317,8 +5321,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5375,8 +5379,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5433,8 +5437,8 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9144</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5453,6 +5457,132 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
+          <a:ext cx="8711565" cy="20320"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path w="8711565" h="20320">
+              <a:moveTo>
+                <a:pt x="8711184" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="19812"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="8711184" y="19812"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="8711184" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="666666"/>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8711565" cy="20320"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="Shape 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C288488E-CA43-CD45-BB80-C8C180FABDAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3153475" y="0"/>
+          <a:ext cx="8711565" cy="20320"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path w="8711565" h="20320">
+              <a:moveTo>
+                <a:pt x="8711184" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="19812"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="8711184" y="19812"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="8711184" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="666666"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>	</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8711565" cy="20320"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="Shape 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CBA7692-F0AF-F94D-8888-FBE848ED3D69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3305875" y="152400"/>
           <a:ext cx="8711565" cy="20320"/>
         </a:xfrm>
         <a:custGeom>
@@ -5813,432 +5943,590 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2594111.4500000007</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>269803.90999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2982282.9000000004</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1443421.6000000003</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>10870450.410000002</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1639524.4399999997</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1322623.1400000004</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>531234.80999999994</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>149877.96000000002</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>8156988.6500000013</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3922231.39</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3">
+        <v>366379.15</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3">
+        <v>639358.13000000012</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3150714.7399999998</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2507824.44</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3">
+        <v>663798.59</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1081566.75</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>2061802.99</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1798769.9</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3">
+        <v>454207.9499999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2527028.4499999993</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1945683.42</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4229591.92</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1175803.4599999997</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1057267.53</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2381459.5599999996</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="3">
+        <v>358173.08</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="3">
+        <v>438604.36000000004</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1356340.3199999998</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="3">
+        <v>487388.72000000003</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2952241.9099999997</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3">
+        <v>779954.07</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3">
+        <v>5655159.9799999995</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4090570.06</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="3">
+        <v>155141.85000000003</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3414996.1099999994</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="3">
+        <v>2228735.64</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1549006.88</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="3">
+        <v>5244499.0900000008</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3">
+        <v>411445.17</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2140550.7799999998</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="3">
+        <v>186466.03</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3">
+        <v>3609882.0799999991</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="3">
+        <v>8870467.7999999989</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1190136.4500000002</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3">
+        <v>225861.03999999998</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="3">
+        <v>2329064.0399999996</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2505790.7899999996</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B50" s="3">
+        <v>778109.8899999999</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="B51" s="3">
+        <v>1649070.5299999998</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2594111.4500000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>269803.90999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2982282.9000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1443421.6000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>10870450.410000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1639524.4399999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1322623.1400000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>531234.80999999994</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>149877.96000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>8156988.6500000013</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3922231.39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>366379.15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>639358.13000000012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3150714.7399999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2507824.44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2">
-        <v>663798.59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1081566.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
-        <v>2061802.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1798769.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2">
-        <v>454207.9499999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2527028.4499999993</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1945683.42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2">
-        <v>4229591.92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1175803.4599999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2">
-        <v>1057267.53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="2">
-        <v>2381459.5599999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="2">
-        <v>358173.08</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2">
-        <v>438604.36000000004</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1356340.3199999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="2">
-        <v>487388.72000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2">
-        <v>2952241.9099999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2">
-        <v>779954.07</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2">
-        <v>5655159.9799999995</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="2">
-        <v>4090570.06</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2">
-        <v>155141.85000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2">
-        <v>3414996.1099999994</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="2">
-        <v>2228735.64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="2">
-        <v>1549006.88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2">
-        <v>5244499.0900000008</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="2">
-        <v>411445.17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2">
-        <v>2140550.7799999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="2">
-        <v>186466.03</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="2">
-        <v>3609882.0799999991</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="2">
-        <v>8870467.7999999989</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1190136.4500000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="2">
-        <v>225861.03999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2329064.0399999996</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="2">
-        <v>2505790.7899999996</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="2">
-        <v>778109.8899999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1649070.5299999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="2">
+    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="3">
         <v>190459.73</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>